<commit_message>
ADD-on done and the final visual of the sheet
</commit_message>
<xml_diff>
--- a/usage_report.xlsx
+++ b/usage_report.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0&quot; GB&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00&quot; EGP&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -31,12 +32,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -57,7 +64,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -68,7 +75,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -79,14 +92,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFF00"/>
+          <fgColor rgb="00FF0000"/>
+          <bgColor rgb="00FF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FF0000"/>
+          <fgColor rgb="00FFFF00"/>
+          <bgColor rgb="00FFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -452,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,20 +493,35 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
+          <t>Total Cost</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Renewal Cost</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Add-ons Price</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Add-ons</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
           <t>Main Quota</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Remaining</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Renewal Cost</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>Renewal Date</t>
         </is>
@@ -508,23 +538,30 @@
           <t>0237613761</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>680 EGP</t>
-        </is>
+      <c r="C2" s="4" t="n">
+        <v>680.71</v>
       </c>
       <c r="D2" s="4" t="n">
+        <v>580</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="n">
         <v>400</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <v>184.05</v>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>570 EGP</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="I2" s="5" t="n">
+        <v>169.74</v>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>17-06-2025</t>
         </is>
@@ -541,23 +578,30 @@
           <t>0237621888</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>281 EGP</t>
-        </is>
+      <c r="C3" s="4" t="n">
+        <v>281.77</v>
       </c>
       <c r="D3" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E3" s="4" t="n">
-        <v>139.75</v>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="I3" s="5" t="n">
+        <v>139.74</v>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
         <is>
           <t>26-06-2025</t>
         </is>
@@ -574,23 +618,30 @@
           <t>0225194422</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>219 EGP</t>
-        </is>
+      <c r="C4" s="6" t="n">
+        <v>219.31</v>
       </c>
       <c r="D4" s="4" t="n">
+        <v>580</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="n">
         <v>400</v>
       </c>
-      <c r="E4" s="4" t="n">
-        <v>380.63</v>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>570 EGP</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="I4" s="5" t="n">
+        <v>363.39</v>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
         <is>
           <t>28-06-2025</t>
         </is>
@@ -607,23 +658,30 @@
           <t>0225194441</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>412 EGP</t>
-        </is>
+      <c r="C5" s="4" t="n">
+        <v>412.81</v>
       </c>
       <c r="D5" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="I5" s="5" t="n">
         <v>133.94</v>
       </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
+      <c r="J5" s="3" t="inlineStr">
         <is>
           <t>16-06-2025</t>
         </is>
@@ -640,23 +698,30 @@
           <t>0222701186</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>495 EGP</t>
-        </is>
+      <c r="C6" s="4" t="n">
+        <v>495.45</v>
       </c>
       <c r="D6" s="4" t="n">
+        <v>360</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>360</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="n">
         <v>250</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="I6" s="5" t="n">
         <v>144.63</v>
       </c>
-      <c r="F6" s="3" t="inlineStr">
-        <is>
-          <t>360 EGP</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
+      <c r="J6" s="3" t="inlineStr">
         <is>
           <t>14-06-2025</t>
         </is>
@@ -673,23 +738,30 @@
           <t>0222716555</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>315 EGP</t>
-        </is>
+      <c r="C7" s="4" t="n">
+        <v>315.09</v>
       </c>
       <c r="D7" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="I7" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
+      <c r="J7" s="3" t="inlineStr">
         <is>
           <t>28-06-2025</t>
         </is>
@@ -706,23 +778,30 @@
           <t>0227764017</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>750 EGP</t>
-        </is>
+      <c r="C8" s="4" t="n">
+        <v>750.71</v>
       </c>
       <c r="D8" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="n">
         <v>400</v>
       </c>
-      <c r="E8" s="4" t="n">
-        <v>230.33</v>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>570 EGP</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
+      <c r="I8" s="5" t="n">
+        <v>224.92</v>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
         <is>
           <t>15-06-2025</t>
         </is>
@@ -739,23 +818,30 @@
           <t>0227764555</t>
         </is>
       </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>266 EGP</t>
-        </is>
+      <c r="C9" s="4" t="n">
+        <v>266.33</v>
       </c>
       <c r="D9" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E9" s="4" t="n">
-        <v>137.24</v>
-      </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
+      <c r="I9" s="5" t="n">
+        <v>136.88</v>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
         <is>
           <t>25-06-2025</t>
         </is>
@@ -772,23 +858,30 @@
           <t>0238860542</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>1267 EGP</t>
-        </is>
+      <c r="C10" s="4" t="n">
+        <v>1267.54</v>
       </c>
       <c r="D10" s="4" t="n">
+        <v>580</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="n">
         <v>400</v>
       </c>
-      <c r="E10" s="4" t="n">
-        <v>53.38</v>
-      </c>
-      <c r="F10" s="3" t="inlineStr">
-        <is>
-          <t>570 EGP</t>
-        </is>
-      </c>
-      <c r="G10" s="3" t="inlineStr">
+      <c r="I10" s="5" t="n">
+        <v>53.23</v>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
         <is>
           <t>08-06-2025</t>
         </is>
@@ -805,23 +898,30 @@
           <t>0238860008</t>
         </is>
       </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>604 EGP</t>
-        </is>
+      <c r="C11" s="4" t="n">
+        <v>604.39</v>
       </c>
       <c r="D11" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E11" s="4" t="n">
-        <v>114.89</v>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G11" s="3" t="inlineStr">
+      <c r="I11" s="5" t="n">
+        <v>113.91</v>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
         <is>
           <t>16-06-2025</t>
         </is>
@@ -838,23 +938,30 @@
           <t>0226948820</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>359 EGP</t>
-        </is>
+      <c r="C12" s="4" t="n">
+        <v>359.3</v>
       </c>
       <c r="D12" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="I12" s="5" t="n">
         <v>139.28</v>
       </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="inlineStr">
+      <c r="J12" s="3" t="inlineStr">
         <is>
           <t>25-06-2025</t>
         </is>
@@ -871,23 +978,30 @@
           <t>0225641141</t>
         </is>
       </c>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>587 EGP</t>
-        </is>
+      <c r="C13" s="6" t="n">
+        <v>587.38</v>
       </c>
       <c r="D13" s="4" t="n">
+        <v>595</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>FTTH Rental ONT</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="n">
         <v>400</v>
       </c>
-      <c r="E13" s="4" t="n">
-        <v>350.4</v>
-      </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>570 EGP</t>
-        </is>
-      </c>
-      <c r="G13" s="3" t="inlineStr">
+      <c r="I13" s="5" t="n">
+        <v>340.74</v>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
         <is>
           <t>26-06-2025</t>
         </is>
@@ -904,23 +1018,30 @@
           <t>0225603344</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>375 EGP</t>
-        </is>
+      <c r="C14" s="4" t="n">
+        <v>375.97</v>
       </c>
       <c r="D14" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="I14" s="5" t="n">
         <v>139.9</v>
       </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
+      <c r="J14" s="3" t="inlineStr">
         <is>
           <t>21-06-2025</t>
         </is>
@@ -937,23 +1058,30 @@
           <t>0238863423</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>2958 EGP</t>
-        </is>
+      <c r="C15" s="4" t="n">
+        <v>2958.08</v>
       </c>
       <c r="D15" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" s="5" t="n">
         <v>400</v>
       </c>
-      <c r="E15" s="4" t="n">
-        <v>36.89</v>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>570 EGP</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
+      <c r="I15" s="5" t="n">
+        <v>21.88</v>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
         <is>
           <t>16-06-2025</t>
         </is>
@@ -970,23 +1098,30 @@
           <t>0238573447</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>585 EGP</t>
-        </is>
+      <c r="C16" s="4" t="n">
+        <v>585.27</v>
       </c>
       <c r="D16" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H16" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E16" s="4" t="n">
-        <v>112.98</v>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
+      <c r="I16" s="5" t="n">
+        <v>111.84</v>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
         <is>
           <t>12-06-2025</t>
         </is>
@@ -1003,23 +1138,30 @@
           <t>0235391499</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>481 EGP</t>
-        </is>
+      <c r="C17" s="4" t="n">
+        <v>481.93</v>
       </c>
       <c r="D17" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H17" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E17" s="4" t="n">
-        <v>125.47</v>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr">
+      <c r="I17" s="5" t="n">
+        <v>124.84</v>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
         <is>
           <t>10-06-2025</t>
         </is>
@@ -1036,23 +1178,30 @@
           <t>0238379383</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>1215 EGP</t>
-        </is>
+      <c r="C18" s="4" t="n">
+        <v>1215.27</v>
       </c>
       <c r="D18" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>570</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" s="5" t="n">
         <v>400</v>
       </c>
-      <c r="E18" s="4" t="n">
-        <v>189.48</v>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
-        <is>
-          <t>570 EGP</t>
-        </is>
-      </c>
-      <c r="G18" s="3" t="inlineStr">
+      <c r="I18" s="5" t="n">
+        <v>181.34</v>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
         <is>
           <t>13-06-2025</t>
         </is>
@@ -1069,23 +1218,30 @@
           <t>0238355580</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>548 EGP</t>
-        </is>
+      <c r="C19" s="4" t="n">
+        <v>548.08</v>
       </c>
       <c r="D19" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>PREMIUM Router</t>
+        </is>
+      </c>
+      <c r="H19" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E19" s="4" t="n">
-        <v>135.84</v>
-      </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G19" s="3" t="inlineStr">
+      <c r="I19" s="5" t="n">
+        <v>135.76</v>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
         <is>
           <t>16-06-2025</t>
         </is>
@@ -1102,35 +1258,42 @@
           <t>0225331143</t>
         </is>
       </c>
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>387 EGP</t>
-        </is>
+      <c r="C20" s="4" t="n">
+        <v>387.91</v>
       </c>
       <c r="D20" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H20" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="E20" s="4" t="n">
-        <v>139.21</v>
-      </c>
-      <c r="F20" s="3" t="inlineStr">
-        <is>
-          <t>210 EGP</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="inlineStr">
+      <c r="I20" s="5" t="n">
+        <v>139.2</v>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
         <is>
           <t>25-06-2025</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E20">
-    <cfRule type="cellIs" priority="1" operator="lessThan" dxfId="0">
+  <conditionalFormatting sqref="I2:I20">
+    <cfRule type="cellIs" priority="1" operator="lessThan" dxfId="0" stopIfTrue="1">
+      <formula>20.0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="1" stopIfTrue="1">
       <formula>80.0</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="1">
-      <formula>20.0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Final Slack-integration ISA xD
</commit_message>
<xml_diff>
--- a/usage_report.xlsx
+++ b/usage_report.xlsx
@@ -545,7 +545,7 @@
         <v>400</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>158.6</v>
+        <v>153.09</v>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         <v>140</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>139.65</v>
+        <v>139.64</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
         <v>400</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>350.07</v>
+        <v>343.35</v>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
@@ -785,7 +785,7 @@
         <v>400</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>219.4</v>
+        <v>215.74</v>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
@@ -825,7 +825,7 @@
         <v>140</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>136.55</v>
+        <v>136.27</v>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
         <v>400</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>53.07</v>
+        <v>52.98</v>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
@@ -905,7 +905,7 @@
         <v>140</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>112.82</v>
+        <v>112.47</v>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         <v>140</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>139.28</v>
+        <v>139.25</v>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>400</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>329.82</v>
+        <v>319.38</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
@@ -1065,7 +1065,7 @@
         <v>400</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>396.44</v>
+        <v>383.15</v>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
         <v>140</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>110.47</v>
+        <v>110.07</v>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
@@ -1145,7 +1145,7 @@
         <v>140</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>124.64</v>
+        <v>124.23</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
@@ -1185,7 +1185,7 @@
         <v>400</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>172.26</v>
+        <v>166.3</v>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
@@ -1225,7 +1225,7 @@
         <v>140</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>135.73</v>
+        <v>135.66</v>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
@@ -1265,7 +1265,7 @@
         <v>140</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>139.19</v>
+        <v>139.18</v>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>

</xml_diff>